<commit_message>
data_processing.r updates and readme additions
</commit_message>
<xml_diff>
--- a/Alternative stimulus files/stimuli.xlsx
+++ b/Alternative stimulus files/stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27226"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -22,31 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
-  <si>
-    <t>categoryA_stimuli</t>
-  </si>
-  <si>
-    <t>categoryB_stimuli</t>
-  </si>
-  <si>
-    <t>categoryC_stimuli</t>
-  </si>
-  <si>
-    <t>categoryD_stimuli</t>
-  </si>
-  <si>
-    <t>categoryA_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryB_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryC_image_stimuli</t>
-  </si>
-  <si>
-    <t>categoryD_image_stimuli</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>flower1.jpg</t>
   </si>
@@ -57,22 +33,73 @@
     <t>flower3.jpg</t>
   </si>
   <si>
+    <t>insect1.jpg</t>
+  </si>
+  <si>
+    <t>insect2.jpg</t>
+  </si>
+  <si>
+    <t>insect3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>labelA_stimuli</t>
+  </si>
+  <si>
+    <t>labelB_stimuli</t>
+  </si>
+  <si>
+    <t>targetA_stimuli</t>
+  </si>
+  <si>
+    <t>targetB_stimuli</t>
+  </si>
+  <si>
+    <t>labelA_image_stimuli</t>
+  </si>
+  <si>
+    <t>labelB_image_stimuli</t>
+  </si>
+  <si>
+    <t>targetA_image_stimuli</t>
+  </si>
+  <si>
+    <t>targetB_image_stimuli</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>friendly</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>pretty</t>
+  </si>
+  <si>
+    <t>hostile</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>hateful</t>
+  </si>
+  <si>
     <t>flower4.jpg</t>
   </si>
   <si>
-    <t>insect1.jpg</t>
-  </si>
-  <si>
-    <t>insect2.jpg</t>
-  </si>
-  <si>
-    <t>insect3.jpg</t>
-  </si>
-  <si>
     <t>insect4.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>blank.jpg</t>
   </si>
 </sst>
 </file>
@@ -114,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="705">
+  <cellStyleXfs count="707">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,12 +847,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="705">
+  <cellStyles count="707">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1178,6 +1208,7 @@
     <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1530,6 +1561,7 @@
     <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1860,7 +1892,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1874,236 +1906,206 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>